<commit_message>
update docker-compose with celery
</commit_message>
<xml_diff>
--- a/app/admin/Menu.xlsx
+++ b/app/admin/Menu.xlsx
@@ -182,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -203,6 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -421,10 +422,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -437,7 +438,7 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -451,7 +452,7 @@
       <c r="E1" s="8"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="1">
         <v>1</v>
@@ -465,7 +466,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="3">
@@ -480,8 +481,11 @@
       <c r="F3" s="4">
         <v>182.99</v>
       </c>
+      <c r="G3" s="10">
+        <v>0.4</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1">
+    <row r="4" spans="1:7" ht="16.5" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3">
@@ -497,7 +501,7 @@
         <v>215.36</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3">
@@ -513,7 +517,7 @@
         <v>265.57</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="1">
         <v>2</v>
@@ -527,7 +531,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1">
@@ -543,7 +547,7 @@
         <v>166.47</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1">
@@ -559,7 +563,7 @@
         <v>168.25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1">
@@ -575,7 +579,7 @@
         <v>132.88</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="5">
         <v>2</v>
       </c>
@@ -589,7 +593,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="1">
         <v>1</v>
@@ -603,7 +607,7 @@
       <c r="E11" s="7"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="3">
@@ -619,7 +623,7 @@
         <v>2700.79</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="C13" s="3">
@@ -635,7 +639,7 @@
         <v>3100.33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3">
@@ -651,7 +655,7 @@
         <v>1850.42</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="1">
         <v>2</v>
@@ -665,7 +669,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1">

</xml_diff>

<commit_message>
add new endpoint tests
</commit_message>
<xml_diff>
--- a/app/admin/Menu.xlsx
+++ b/app/admin/Menu.xlsx
@@ -33,9 +33,6 @@
     <t>К пиву</t>
   </si>
   <si>
-    <t>Сельдь Бисмарк</t>
-  </si>
-  <si>
     <t>Традиционное немецкое блюдо из маринованной сельди</t>
   </si>
   <si>
@@ -51,12 +48,6 @@
     <t>Рамен</t>
   </si>
   <si>
-    <t>Горячий рамен</t>
-  </si>
-  <si>
-    <t>Дайзу рамен</t>
-  </si>
-  <si>
     <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
   </si>
   <si>
@@ -84,9 +75,6 @@
     <t>Для романтичного вечера</t>
   </si>
   <si>
-    <t>Шемен де Пап ля Ноблесс</t>
-  </si>
-  <si>
     <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
   </si>
   <si>
@@ -127,6 +115,18 @@
   </si>
   <si>
     <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
+  </si>
+  <si>
+    <t>Сельдь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Горячий </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дайзу </t>
+  </si>
+  <si>
+    <t>Шем ля Ноблесс</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A6" sqref="A6:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -473,10 +473,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>5</v>
       </c>
       <c r="F3" s="4">
         <v>182.99</v>
@@ -492,10 +492,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F4" s="4">
         <v>215.36</v>
@@ -508,10 +508,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="F5" s="4">
         <v>265.57</v>
@@ -523,10 +523,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="2"/>
@@ -538,10 +538,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1">
         <v>166.47</v>
@@ -554,10 +554,10 @@
         <v>2</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F8" s="1">
         <v>168.25</v>
@@ -570,10 +570,10 @@
         <v>3</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F9" s="1">
         <v>132.88</v>
@@ -584,10 +584,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7"/>
@@ -599,10 +599,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="2"/>
@@ -614,10 +614,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F12" s="1">
         <v>2700.79</v>
@@ -630,10 +630,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F13" s="1">
         <v>3100.33</v>
@@ -646,10 +646,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F14" s="1">
         <v>1850.42</v>
@@ -661,10 +661,10 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="2"/>
@@ -676,10 +676,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F16" s="1">
         <v>420.78</v>
@@ -692,10 +692,10 @@
         <v>2</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F17" s="1">
         <v>440.11</v>
@@ -708,10 +708,10 @@
         <v>3</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F18" s="1">
         <v>520.08000000000004</v>

</xml_diff>